<commit_message>
UF-6721 - Migrate PR3 data
Adds a validation of legal id check digit ("kontrollsiffra")
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Work/api-service-party-assets/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F17A0EF-6378-AC4B-A66E-FB4E227E668D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4E86AF-396B-8A40-9717-4C9918D554E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1180" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -135,15 +135,6 @@
     <t>OLLE</t>
   </si>
   <si>
-    <t>420330-8948</t>
-  </si>
-  <si>
-    <t>450627-8831</t>
-  </si>
-  <si>
-    <t>550717-7832</t>
-  </si>
-  <si>
     <t>GATAN 12</t>
   </si>
   <si>
@@ -172,6 +163,15 @@
   </si>
   <si>
     <t>Anki Borg</t>
+  </si>
+  <si>
+    <t>550717-7839</t>
+  </si>
+  <si>
+    <t>420330-8947</t>
+  </si>
+  <si>
+    <t>450627-8839</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -689,22 +689,22 @@
         <v>31</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="4">
         <v>39799</v>
@@ -731,10 +731,10 @@
         <v>29</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>28</v>
@@ -775,22 +775,22 @@
         <v>33</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="Q3" s="4">
         <v>39799</v>
@@ -817,7 +817,7 @@
         <v>29</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>28</v>
@@ -861,22 +861,22 @@
         <v>35</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="Q4" s="4">
         <v>40135</v>
@@ -903,7 +903,7 @@
         <v>29</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
UF-17724: Fix for PR3 import regarding Ange
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Work/api-service-party-assets/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kje26wal\work\api-service-party-assets\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EC9A77-B0EE-AF44-B13C-DEB8A2E43C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D523721-9C9C-4881-945F-EAE915357473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="1440" windowWidth="41400" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>ID_KORT</t>
   </si>
@@ -147,9 +147,6 @@
     <t>123 45 STADEN</t>
   </si>
   <si>
-    <t>012-345678</t>
-  </si>
-  <si>
     <t>08/2514</t>
   </si>
   <si>
@@ -165,13 +162,34 @@
     <t>Anki Borg</t>
   </si>
   <si>
-    <t>550717-7839</t>
-  </si>
-  <si>
-    <t>420330-8947</t>
-  </si>
-  <si>
     <t>450627-8838</t>
+  </si>
+  <si>
+    <t>JANNE</t>
+  </si>
+  <si>
+    <t>VÄGEN 35</t>
+  </si>
+  <si>
+    <t>100108-2393</t>
+  </si>
+  <si>
+    <t>070-1740635</t>
+  </si>
+  <si>
+    <t>070-1740636</t>
+  </si>
+  <si>
+    <t>070-1740637</t>
+  </si>
+  <si>
+    <t>070-1740638</t>
+  </si>
+  <si>
+    <t>250107-2389</t>
+  </si>
+  <si>
+    <t>000111-2382</t>
   </si>
 </sst>
 </file>
@@ -181,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +216,12 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -255,11 +279,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,9 +301,14 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{0E414497-5A21-4D02-A472-FCF992D74DC3}"/>
     <cellStyle name="Normal_Blad1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -557,21 +587,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="13.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>123</v>
       </c>
@@ -689,7 +720,7 @@
         <v>31</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>28</v>
@@ -701,10 +732,10 @@
         <v>39</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q2" s="4">
         <v>39799</v>
@@ -731,10 +762,10 @@
         <v>29</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>28</v>
@@ -743,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>456</v>
       </c>
@@ -774,8 +805,8 @@
       <c r="J3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>47</v>
+      <c r="K3" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>28</v>
@@ -787,10 +818,10 @@
         <v>39</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="4">
         <v>39799</v>
@@ -817,7 +848,7 @@
         <v>29</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>28</v>
@@ -829,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>789</v>
       </c>
@@ -861,7 +892,7 @@
         <v>35</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>28</v>
@@ -873,10 +904,10 @@
         <v>39</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q4" s="4">
         <v>40135</v>
@@ -903,15 +934,101 @@
         <v>29</v>
       </c>
       <c r="Y4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2">
+        <v>622</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>80704</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>39799</v>
+      </c>
+      <c r="R5" s="4">
+        <v>39799</v>
+      </c>
+      <c r="S5" s="4">
+        <v>40877</v>
+      </c>
+      <c r="T5" s="4">
+        <v>39799</v>
+      </c>
+      <c r="U5" s="4">
+        <v>39799</v>
+      </c>
+      <c r="V5" s="4">
+        <v>39799</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Z4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB4" s="2">
+      <c r="Z5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB5" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>